<commit_message>
CHORE: Puting branch up to date.
</commit_message>
<xml_diff>
--- a/data/raw/Pending/cápitas-régimen-contributivo-sfs-afiliado-mes-dispersión-2012-2023.xlsx
+++ b/data/raw/Pending/cápitas-régimen-contributivo-sfs-afiliado-mes-dispersión-2012-2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afe3eca1c425187e/Escritorio/Proyecto Humano/data/Raw Data/Pending/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afe3eca1c425187e/Escritorio/Proyecto Humano/data/raw/Pending/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{068F7E83-B4F0-4933-BC4B-FB5D44D88C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D327297A-A3F4-4F2F-80C6-1467D6417EAB}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{068F7E83-B4F0-4933-BC4B-FB5D44D88C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95D1FF7B-7DE5-4B64-BE35-21EA51DCFCCC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9841,20 +9841,22 @@
   <dimension ref="A1:K145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A146" sqref="A146:XFD146"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="1"/>
     <col min="12" max="13" width="11.42578125" style="1" customWidth="1"/>
     <col min="14" max="15" width="11.42578125" style="1"/>

</xml_diff>